<commit_message>
Added Tax List and change the after tax price calculation
</commit_message>
<xml_diff>
--- a/AA_Calculator.xlsx
+++ b/AA_Calculator.xlsx
@@ -1,19 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Github\AA_Calculator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19030D0C-3CFC-476C-9AFA-F5A888491824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="_Example_20231110_Costco - 2023" sheetId="2" r:id="rId5"/>
-    <sheet name="_Example_20231115_Japas - 20231" sheetId="3" r:id="rId6"/>
+    <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Tax List" sheetId="4" r:id="rId2"/>
+    <sheet name="_Example_20231110_Costco - 2023" sheetId="2" r:id="rId3"/>
+    <sheet name="_Example_20231115_Japas - 20231" sheetId="3" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -69,9 +92,6 @@
     <t xml:space="preserve"> MILKIS                </t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>Ming,Eric</t>
   </si>
   <si>
@@ -117,55 +137,63 @@
     <t xml:space="preserve"> PUMA BOXER           </t>
   </si>
   <si>
+    <t>[Example]20231115_Japas</t>
+  </si>
+  <si>
+    <t>20231115_Japas</t>
+  </si>
+  <si>
+    <t>_Example_20231115_Japas - 20231</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Ming, OnLai</t>
+  </si>
+  <si>
+    <t>Udon</t>
+  </si>
+  <si>
+    <t>Apple Royal</t>
+  </si>
+  <si>
+    <t>Tips:</t>
+  </si>
+  <si>
+    <t>List of payee:</t>
+  </si>
+  <si>
+    <t>OnLai</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tax List</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
     <t>LipStick</t>
-  </si>
-  <si>
-    <t>[Example]20231115_Japas</t>
-  </si>
-  <si>
-    <t>20231115_Japas</t>
-  </si>
-  <si>
-    <t>_Example_20231115_Japas - 20231</t>
-  </si>
-  <si>
-    <t>Cat</t>
-  </si>
-  <si>
-    <t>Mayo</t>
-  </si>
-  <si>
-    <t>Food</t>
-  </si>
-  <si>
-    <t>Ming, OnLai</t>
-  </si>
-  <si>
-    <t>Udon</t>
-  </si>
-  <si>
-    <t>Apple Royal</t>
-  </si>
-  <si>
-    <t>Tips:</t>
-  </si>
-  <si>
-    <t>List of payee:</t>
-  </si>
-  <si>
-    <t>OnLai</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="[$CAD]0.00"/>
-    <numFmt numFmtId="60" formatCode="[$CAD]0.00;[Red][$CAD]0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="[$CAD]0.00"/>
+    <numFmt numFmtId="177" formatCode="[$CAD]0.00;[Red][$CAD]0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -182,25 +210,25 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="12"/>
       <color indexed="11"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -216,10 +244,30 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="16"/>
       <color indexed="16"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="6">
@@ -254,7 +302,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -367,168 +415,246 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="43">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="8" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="1" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="8" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="1" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="8" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ff5e88b1"/>
-      <rgbColor rgb="ffeef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ff000018"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FF5E88B1"/>
+      <rgbColor rgb="FFEEF3F4"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FF000018"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -727,7 +853,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -745,7 +871,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -774,7 +900,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -799,7 +925,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -824,7 +950,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -849,7 +975,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -874,7 +1000,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -899,7 +1025,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -924,7 +1050,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -949,7 +1075,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -974,7 +1100,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -987,9 +1113,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1006,7 +1138,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1024,7 +1156,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1049,7 +1181,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1074,7 +1206,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1099,7 +1231,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1124,7 +1256,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1149,7 +1281,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1174,7 +1306,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1199,7 +1331,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1224,7 +1356,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1249,7 +1381,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1262,9 +1394,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1278,7 +1416,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1296,7 +1434,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1325,7 +1463,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1350,7 +1488,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1375,7 +1513,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1400,7 +1538,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1425,7 +1563,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1450,7 +1588,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1475,7 +1613,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1500,7 +1638,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1525,7 +1663,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1538,866 +1676,941 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="2" max="4" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="0.05" customHeight="1">
-      <c r="B3" t="s" s="1">
+    <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1">
+      <c r="B3" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+    </row>
+    <row r="7" spans="2:4" ht="17.399999999999999">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+    <row r="9" spans="2:4" ht="15">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="2:4" ht="30">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="D10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" t="s" s="3">
+    <row r="11" spans="2:4" ht="15">
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:4" ht="30">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
-      <c r="C12" t="s" s="4">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s" s="5">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D10" location="'_Example_20231110_Costco - 2023'!R2C1" tooltip="" display="_Example_20231110_Costco - 2023"/>
-    <hyperlink ref="D12" location="'_Example_20231115_Japas - 20231'!R2C1" tooltip="" display="_Example_20231115_Japas - 20231"/>
+    <hyperlink ref="D10" location="'_Example_20231110_Costco - 2023'!R2C1" display="_Example_20231110_Costco - 2023" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D12" location="'_Example_20231115_Japas - 20231'!R2C1" display="_Example_20231115_Japas - 20231" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:K16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDF181E-13F2-43B0-A9C7-2028A2DF9FCD}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="20.3672" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="6" customWidth="1"/>
-    <col min="3" max="3" width="5.22656" style="6" customWidth="1"/>
-    <col min="4" max="11" width="16.3516" style="6" customWidth="1"/>
-    <col min="12" max="16384" width="16.3516" style="6" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="7">
+    <row r="1" spans="1:2" ht="14.4" thickBot="1">
+      <c r="A1" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="41">
+        <v>0.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" style="5" customWidth="1"/>
+    <col min="4" max="12" width="16.33203125" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="16.33203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="27.6" customHeight="1">
+      <c r="A1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" ht="23.2" customHeight="1">
-      <c r="A2" t="s" s="8">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+    </row>
+    <row r="2" spans="1:11" ht="23.25" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="9">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="8">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="10">
+      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="8">
+      <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="8">
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s" s="8">
+      <c r="G2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" ht="27.55" customHeight="1">
-      <c r="A3" t="s" s="12">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" ht="27.6" customHeight="1">
+      <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="13">
-        <v>16.49</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15">
-        <f>IF(C3="H",ROUND(B3*J$3,2),B3)</f>
-        <v>16.49</v>
-      </c>
-      <c r="E3" t="s" s="16">
+      <c r="B3" s="11">
+        <v>16.489999999999998</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="13">
+        <f>IF(C3&lt;&gt;"",ROUND(B3*(VLOOKUP(C3, 'Tax List'!A:B, 2,FALSE)+1),2),B3)</f>
+        <v>18.63</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="17">
-        <f>IF(E3="ALL",J$4,LEN(TRIM(E3))-LEN(SUBSTITUTE(TRIM(E3),",",""))+1)</f>
+      <c r="F3" s="15">
+        <f t="shared" ref="F3:F14" si="0">IF(E3="ALL",J$4,LEN(TRIM(E3))-LEN(SUBSTITUTE(TRIM(E3),",",""))+1)</f>
         <v>1</v>
       </c>
-      <c r="G3" s="18">
-        <f>D3/F3</f>
-        <v>16.49</v>
-      </c>
-      <c r="H3" s="14"/>
-      <c r="I3" t="s" s="19">
+      <c r="G3" s="16">
+        <f t="shared" ref="G3:G13" si="1">D3/F3</f>
+        <v>18.63</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="12"/>
+    </row>
+    <row r="4" spans="1:11" ht="27.3" customHeight="1">
+      <c r="A4" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="20">
+        <v>15.99</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="20">
-        <v>1.13</v>
-      </c>
-      <c r="K3" s="14"/>
-    </row>
-    <row r="4" ht="27.35" customHeight="1">
-      <c r="A4" t="s" s="21">
-        <v>17</v>
-      </c>
-      <c r="B4" s="22">
-        <v>15.99</v>
-      </c>
-      <c r="C4" t="s" s="23">
+      <c r="D4" s="13">
+        <f>IF(C4&lt;&gt;"",ROUND(B4*(VLOOKUP(C4, 'Tax List'!A:B, 2,FALSE)+1),2),B4)</f>
+        <v>18.07</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="24">
-        <f>IF(C4="H",ROUND(B4*J$3,2),B4)</f>
-        <v>18.07</v>
-      </c>
-      <c r="E4" t="s" s="25">
+      <c r="F4" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G4" s="25">
+        <f t="shared" si="1"/>
+        <v>9.0350000000000001</v>
+      </c>
+      <c r="H4" s="26"/>
+      <c r="I4" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="26">
-        <f>IF(E4="ALL",J$4,LEN(TRIM(E4))-LEN(SUBSTITUTE(TRIM(E4),",",""))+1)</f>
+      <c r="J4" s="27">
+        <v>3</v>
+      </c>
+      <c r="K4" s="26"/>
+    </row>
+    <row r="5" spans="1:11" ht="27.3" customHeight="1">
+      <c r="A5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="20">
+        <v>66.06</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13">
+        <f>IF(C5&lt;&gt;"",ROUND(B5*(VLOOKUP(C5, 'Tax List'!A:B, 2,FALSE)+1),2),B5)</f>
+        <v>66.06</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="24">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G4" s="27">
-        <f>D4/F4</f>
-        <v>9.035</v>
-      </c>
-      <c r="H4" s="28"/>
-      <c r="I4" t="s" s="23">
-        <v>20</v>
-      </c>
-      <c r="J4" s="29">
+      <c r="G5" s="25">
+        <f t="shared" si="1"/>
+        <v>33.03</v>
+      </c>
+      <c r="H5" s="26"/>
+      <c r="I5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="25">
+        <f>SUMIF(E$3:E$14,"ALL",G$3:G$14)+SUMIF(E$3:E$14,"*"&amp;I5&amp;"*",G$3:G$14)</f>
+        <v>147.30833333333331</v>
+      </c>
+      <c r="K5" s="26"/>
+    </row>
+    <row r="6" spans="1:11" ht="27.3" customHeight="1">
+      <c r="A6" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="20">
+        <v>31.99</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13">
+        <f>IF(C6&lt;&gt;"",ROUND(B6*(VLOOKUP(C6, 'Tax List'!A:B, 2,FALSE)+1),2),B6)</f>
+        <v>31.99</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="24">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="K4" s="28"/>
-    </row>
-    <row r="5" ht="27.35" customHeight="1">
-      <c r="A5" t="s" s="21">
-        <v>21</v>
-      </c>
-      <c r="B5" s="22">
-        <v>66.06</v>
-      </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="24">
-        <f>IF(C5="H",ROUND(B5*J$3,2),B5)</f>
-        <v>66.06</v>
-      </c>
-      <c r="E5" t="s" s="25">
-        <v>19</v>
-      </c>
-      <c r="F5" s="26">
-        <f>IF(E5="ALL",J$4,LEN(TRIM(E5))-LEN(SUBSTITUTE(TRIM(E5),",",""))+1)</f>
+      <c r="G6" s="25">
+        <f t="shared" si="1"/>
+        <v>10.663333333333332</v>
+      </c>
+      <c r="H6" s="26"/>
+      <c r="I6" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="25">
+        <f>SUMIF(E$3:E$14,"ALL",G$3:G$14)+SUMIF(E$3:E$14,"*"&amp;I6&amp;"*",G$3:G$14)</f>
+        <v>10.663333333333332</v>
+      </c>
+      <c r="K6" s="26"/>
+    </row>
+    <row r="7" spans="1:11" ht="27.3" customHeight="1">
+      <c r="A7" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="20">
+        <v>44.99</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13">
+        <f>IF(C7&lt;&gt;"",ROUND(B7*(VLOOKUP(C7, 'Tax List'!A:B, 2,FALSE)+1),2),B7)</f>
+        <v>44.99</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="25">
+        <f t="shared" si="1"/>
+        <v>44.99</v>
+      </c>
+      <c r="H7" s="26"/>
+      <c r="I7" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="25">
+        <f>SUMIF(E$3:E$14,"ALL",G$3:G$14)+SUMIF(E$3:E$14,"*"&amp;I7&amp;"*",G$3:G$14)</f>
+        <v>109.45833333333334</v>
+      </c>
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" spans="1:11" ht="27.3" customHeight="1">
+      <c r="A8" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="20">
+        <v>-10</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13">
+        <f>IF(C8&lt;&gt;"",ROUND(B8*(VLOOKUP(C8, 'Tax List'!A:B, 2,FALSE)+1),2),B8)</f>
+        <v>-10</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="25">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="H8" s="26"/>
+      <c r="I8" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="25">
+        <f>SUM(J5,J7,J6)</f>
+        <v>267.43</v>
+      </c>
+      <c r="K8" s="26"/>
+    </row>
+    <row r="9" spans="1:11" ht="27.3" customHeight="1">
+      <c r="A9" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="20">
+        <v>9.99</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="13">
+        <f>IF(C9&lt;&gt;"",ROUND(B9*(VLOOKUP(C9, 'Tax List'!A:B, 2,FALSE)+1),2),B9)</f>
+        <v>11.29</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="25">
+        <f t="shared" si="1"/>
+        <v>11.29</v>
+      </c>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+    </row>
+    <row r="10" spans="1:11" ht="27.3" customHeight="1">
+      <c r="A10" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="20">
+        <v>8.49</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13">
+        <f>IF(C10&lt;&gt;"",ROUND(B10*(VLOOKUP(C10, 'Tax List'!A:B, 2,FALSE)+1),2),B10)</f>
+        <v>8.49</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="24">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G5" s="27">
-        <f>D5/F5</f>
-        <v>33.03</v>
-      </c>
-      <c r="H5" s="28"/>
-      <c r="I5" t="s" s="23">
+      <c r="G10" s="25">
+        <f t="shared" si="1"/>
+        <v>4.2450000000000001</v>
+      </c>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="26"/>
+    </row>
+    <row r="11" spans="1:11" ht="27.3" customHeight="1">
+      <c r="A11" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="20">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="13">
+        <f>IF(C11&lt;&gt;"",ROUND(B11*(VLOOKUP(C11, 'Tax List'!A:B, 2,FALSE)+1),2),B11)</f>
+        <v>22.59</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G11" s="25">
+        <f t="shared" si="1"/>
+        <v>11.295</v>
+      </c>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+    </row>
+    <row r="12" spans="1:11" ht="27.3" customHeight="1">
+      <c r="A12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="20">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="13">
+        <f>IF(C12&lt;&gt;"",ROUND(B12*(VLOOKUP(C12, 'Tax List'!A:B, 2,FALSE)+1),2),B12)</f>
+        <v>20.329999999999998</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="27">
-        <f>SUMIF(E$3:E$14,"ALL",G$3:G$14)+SUMIF(E$3:E$14,"*"&amp;I5&amp;"*",G$3:G$14)</f>
-        <v>145.168333333333</v>
-      </c>
-      <c r="K5" s="28"/>
-    </row>
-    <row r="6" ht="27.35" customHeight="1">
-      <c r="A6" t="s" s="21">
-        <v>22</v>
-      </c>
-      <c r="B6" s="22">
-        <v>31.99</v>
-      </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="24">
-        <f>IF(C6="H",ROUND(B6*J$3,2),B6)</f>
-        <v>31.99</v>
-      </c>
-      <c r="E6" t="s" s="23">
-        <v>23</v>
-      </c>
-      <c r="F6" s="26">
-        <f>IF(E6="ALL",J$4,LEN(TRIM(E6))-LEN(SUBSTITUTE(TRIM(E6),",",""))+1)</f>
-        <v>3</v>
-      </c>
-      <c r="G6" s="27">
-        <f>D6/F6</f>
-        <v>10.6633333333333</v>
-      </c>
-      <c r="H6" s="28"/>
-      <c r="I6" t="s" s="23">
-        <v>24</v>
-      </c>
-      <c r="J6" s="27">
-        <f>SUMIF(E$3:E$14,"ALL",G$3:G$14)+SUMIF(E$3:E$14,"*"&amp;I6&amp;"*",G$3:G$14)</f>
-        <v>10.6633333333333</v>
-      </c>
-      <c r="K6" s="28"/>
-    </row>
-    <row r="7" ht="27.35" customHeight="1">
-      <c r="A7" t="s" s="21">
-        <v>25</v>
-      </c>
-      <c r="B7" s="22">
-        <v>44.99</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="24">
-        <f>IF(C7="H",ROUND(B7*J$3,2),B7)</f>
-        <v>44.99</v>
-      </c>
-      <c r="E7" t="s" s="25">
-        <v>26</v>
-      </c>
-      <c r="F7" s="26">
-        <f>IF(E7="ALL",J$4,LEN(TRIM(E7))-LEN(SUBSTITUTE(TRIM(E7),",",""))+1)</f>
+      <c r="F12" s="24">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G7" s="27">
-        <f>D7/F7</f>
-        <v>44.99</v>
-      </c>
-      <c r="H7" s="28"/>
-      <c r="I7" t="s" s="23">
-        <v>26</v>
-      </c>
-      <c r="J7" s="27">
-        <f>SUMIF(E$3:E$14,"ALL",G$3:G$14)+SUMIF(E$3:E$14,"*"&amp;I7&amp;"*",G$3:G$14)</f>
-        <v>109.458333333333</v>
-      </c>
-      <c r="K7" s="28"/>
-    </row>
-    <row r="8" ht="27.35" customHeight="1">
-      <c r="A8" t="s" s="21">
+      <c r="G12" s="25">
+        <f t="shared" si="1"/>
+        <v>20.329999999999998</v>
+      </c>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+    </row>
+    <row r="13" spans="1:11" ht="27.3" customHeight="1">
+      <c r="A13" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="20">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="13">
+        <f>IF(C13&lt;&gt;"",ROUND(B13*(VLOOKUP(C13, 'Tax List'!A:B, 2,FALSE)+1),2),B13)</f>
+        <v>22.59</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="25">
+        <f t="shared" si="1"/>
+        <v>22.59</v>
+      </c>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+    </row>
+    <row r="14" spans="1:11" ht="27.3" customHeight="1">
+      <c r="A14" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13">
+        <f>IF(C14&lt;&gt;"",ROUND(B14*(VLOOKUP(C14, 'Tax List'!A:B, 2,FALSE)+1),2),B14)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G14" s="28">
+        <v>6.2</v>
+      </c>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+    </row>
+    <row r="15" spans="1:11" ht="22.95" customHeight="1">
+      <c r="A15" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="22">
-        <v>-10</v>
-      </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="24">
-        <f>IF(C8="H",ROUND(B8*J$3,2),B8)</f>
-        <v>-10</v>
-      </c>
-      <c r="E8" t="s" s="25">
-        <v>26</v>
-      </c>
-      <c r="F8" s="26">
-        <f>IF(E8="ALL",J$4,LEN(TRIM(E8))-LEN(SUBSTITUTE(TRIM(E8),",",""))+1)</f>
-        <v>1</v>
-      </c>
-      <c r="G8" s="27">
-        <f>D8/F8</f>
-        <v>-10</v>
-      </c>
-      <c r="H8" s="28"/>
-      <c r="I8" t="s" s="23">
-        <v>28</v>
-      </c>
-      <c r="J8" s="27">
-        <f>SUM(J5,J7,J6)</f>
-        <v>265.289999999999</v>
-      </c>
-      <c r="K8" s="28"/>
-    </row>
-    <row r="9" ht="27.35" customHeight="1">
-      <c r="A9" t="s" s="21">
-        <v>29</v>
-      </c>
-      <c r="B9" s="22">
-        <v>9.99</v>
-      </c>
-      <c r="C9" t="s" s="23">
-        <v>18</v>
-      </c>
-      <c r="D9" s="24">
-        <f>IF(C9="H",ROUND(B9*J$3,2),B9)</f>
-        <v>11.29</v>
-      </c>
-      <c r="E9" t="s" s="25">
-        <v>15</v>
-      </c>
-      <c r="F9" s="26">
-        <f>IF(E9="ALL",J$4,LEN(TRIM(E9))-LEN(SUBSTITUTE(TRIM(E9),",",""))+1)</f>
-        <v>1</v>
-      </c>
-      <c r="G9" s="27">
-        <f>D9/F9</f>
-        <v>11.29</v>
-      </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-    </row>
-    <row r="10" ht="27.35" customHeight="1">
-      <c r="A10" t="s" s="21">
-        <v>30</v>
-      </c>
-      <c r="B10" s="22">
-        <v>8.49</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="24">
-        <f>IF(C10="H",ROUND(B10*J$3,2),B10)</f>
-        <v>8.49</v>
-      </c>
-      <c r="E10" t="s" s="25">
-        <v>19</v>
-      </c>
-      <c r="F10" s="26">
-        <f>IF(E10="ALL",J$4,LEN(TRIM(E10))-LEN(SUBSTITUTE(TRIM(E10),",",""))+1)</f>
-        <v>2</v>
-      </c>
-      <c r="G10" s="27">
-        <f>D10/F10</f>
-        <v>4.245</v>
-      </c>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="28"/>
-    </row>
-    <row r="11" ht="27.35" customHeight="1">
-      <c r="A11" t="s" s="21">
-        <v>31</v>
-      </c>
-      <c r="B11" s="22">
-        <v>19.99</v>
-      </c>
-      <c r="C11" t="s" s="23">
-        <v>18</v>
-      </c>
-      <c r="D11" s="24">
-        <f>IF(C11="H",ROUND(B11*J$3,2),B11)</f>
-        <v>22.59</v>
-      </c>
-      <c r="E11" t="s" s="25">
-        <v>19</v>
-      </c>
-      <c r="F11" s="26">
-        <f>IF(E11="ALL",J$4,LEN(TRIM(E11))-LEN(SUBSTITUTE(TRIM(E11),",",""))+1)</f>
-        <v>2</v>
-      </c>
-      <c r="G11" s="27">
-        <f>D11/F11</f>
-        <v>11.295</v>
-      </c>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-    </row>
-    <row r="12" ht="27.35" customHeight="1">
-      <c r="A12" t="s" s="21">
-        <v>32</v>
-      </c>
-      <c r="B12" s="22">
-        <v>17.99</v>
-      </c>
-      <c r="C12" t="s" s="23">
-        <v>18</v>
-      </c>
-      <c r="D12" s="24">
-        <f>IF(C12="H",ROUND(B12*J$3,2),B12)</f>
-        <v>20.33</v>
-      </c>
-      <c r="E12" t="s" s="25">
-        <v>15</v>
-      </c>
-      <c r="F12" s="26">
-        <f>IF(E12="ALL",J$4,LEN(TRIM(E12))-LEN(SUBSTITUTE(TRIM(E12),",",""))+1)</f>
-        <v>1</v>
-      </c>
-      <c r="G12" s="27">
-        <f>D12/F12</f>
-        <v>20.33</v>
-      </c>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-    </row>
-    <row r="13" ht="27.35" customHeight="1">
-      <c r="A13" t="s" s="21">
-        <v>33</v>
-      </c>
-      <c r="B13" s="22">
-        <v>19.99</v>
-      </c>
-      <c r="C13" t="s" s="23">
-        <v>18</v>
-      </c>
-      <c r="D13" s="24">
-        <f>IF(C13="H",ROUND(B13*J$3,2),B13)</f>
-        <v>22.59</v>
-      </c>
-      <c r="E13" t="s" s="25">
-        <v>15</v>
-      </c>
-      <c r="F13" s="26">
-        <f>IF(E13="ALL",J$4,LEN(TRIM(E13))-LEN(SUBSTITUTE(TRIM(E13),",",""))+1)</f>
-        <v>1</v>
-      </c>
-      <c r="G13" s="27">
-        <f>D13/F13</f>
-        <v>22.59</v>
-      </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-    </row>
-    <row r="14" ht="27.35" customHeight="1">
-      <c r="A14" t="s" s="31">
-        <v>34</v>
-      </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="24"/>
-      <c r="E14" t="s" s="25">
-        <v>19</v>
-      </c>
-      <c r="F14" s="26">
-        <f>IF(E14="ALL",J$4,LEN(TRIM(E14))-LEN(SUBSTITUTE(TRIM(E14),",",""))+1)</f>
-        <v>2</v>
-      </c>
-      <c r="G14" s="30">
-        <v>6.2</v>
-      </c>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-    </row>
-    <row r="15" ht="22.95" customHeight="1">
-      <c r="A15" t="s" s="32">
-        <v>28</v>
-      </c>
-      <c r="B15" s="33">
+      <c r="B15" s="30">
         <f>SUM(B3:B14)</f>
-        <v>241.97</v>
-      </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34">
+        <v>241.97000000000006</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31">
         <f>SUM(D3:D14)</f>
-        <v>252.89</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-    </row>
-    <row r="16" ht="22.95" customHeight="1">
-      <c r="A16" s="36"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
+        <v>255.03</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+    </row>
+    <row r="16" spans="1:11" ht="22.95" customHeight="1">
+      <c r="A16" s="33"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{16EC1E25-3802-4899-8871-E904A81DAEB6}">
+          <x14:formula1>
+            <xm:f>'Tax List'!$A$2:$A$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:C14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:L10"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3:K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.3672" style="37" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="37" customWidth="1"/>
-    <col min="3" max="3" width="5.22656" style="37" customWidth="1"/>
-    <col min="4" max="4" width="14.8047" style="37" customWidth="1"/>
-    <col min="5" max="12" width="16.3516" style="37" customWidth="1"/>
-    <col min="13" max="16384" width="16.3516" style="37" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="5" customWidth="1"/>
+    <col min="5" max="13" width="16.33203125" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="16.33203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="7">
+    <row r="1" spans="1:12" ht="27.6" customHeight="1">
+      <c r="A1" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+    </row>
+    <row r="2" spans="1:12" ht="23.25" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-    </row>
-    <row r="2" ht="23.2" customHeight="1">
-      <c r="A2" t="s" s="8">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s" s="8">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s" s="8">
+      <c r="E2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" ht="27.6" customHeight="1">
+      <c r="A3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="11">
+        <v>11</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E2" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s" s="8">
+      <c r="E3" s="13">
+        <f>IF(C3&lt;&gt;"",ROUND(B3*(VLOOKUP(C3, 'Tax List'!A:B, 2,FALSE)+1),2),B3)</f>
+        <v>12.43</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="15">
+        <f t="shared" ref="G3:G8" si="0">IF(F3="ALL",K$4,LEN(TRIM(F3))-LEN(SUBSTITUTE(TRIM(F3),",",""))+1)</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="16">
+        <f t="shared" ref="H3:H8" si="1">E3/G3</f>
+        <v>6.2149999999999999</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="12"/>
+    </row>
+    <row r="4" spans="1:12" ht="27.3" customHeight="1">
+      <c r="A4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="20">
+        <v>17</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="13">
+        <f>IF(C4&lt;&gt;"",ROUND(B4*(VLOOKUP(C4, 'Tax List'!A:B, 2,FALSE)+1),2),B4)</f>
+        <v>19.21</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H4" s="25">
+        <f t="shared" si="1"/>
+        <v>19.21</v>
+      </c>
+      <c r="I4" s="26"/>
+      <c r="J4" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="27">
+        <v>2</v>
+      </c>
+      <c r="L4" s="26"/>
+    </row>
+    <row r="5" spans="1:12" ht="27.3" customHeight="1">
+      <c r="A5" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="20">
         <v>12</v>
       </c>
-      <c r="H2" t="s" s="8">
-        <v>13</v>
-      </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-    </row>
-    <row r="3" ht="27.55" customHeight="1">
-      <c r="A3" t="s" s="12">
-        <v>39</v>
-      </c>
-      <c r="B3" s="13">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s" s="19">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s" s="19">
-        <v>40</v>
-      </c>
-      <c r="E3" s="15">
-        <f>IF(C3="H",ROUND(B3*K$3,2),B3)</f>
-        <v>12.43</v>
-      </c>
-      <c r="F3" t="s" s="16">
-        <v>41</v>
-      </c>
-      <c r="G3" s="17">
-        <f>IF(F3="ALL",K$4,LEN(TRIM(F3))-LEN(SUBSTITUTE(TRIM(F3),",",""))+1)</f>
-        <v>2</v>
-      </c>
-      <c r="H3" s="18">
-        <f>E3/G3</f>
-        <v>6.215</v>
-      </c>
-      <c r="I3" s="14"/>
-      <c r="J3" t="s" s="19">
+      <c r="C5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="20">
-        <v>1.13</v>
-      </c>
-      <c r="L3" s="14"/>
-    </row>
-    <row r="4" ht="27.35" customHeight="1">
-      <c r="A4" t="s" s="21">
+      <c r="D5" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="13">
+        <f>IF(C5&lt;&gt;"",ROUND(B5*(VLOOKUP(C5, 'Tax List'!A:B, 2,FALSE)+1),2),B5)</f>
+        <v>13.56</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H5" s="25">
+        <f t="shared" si="1"/>
+        <v>13.56</v>
+      </c>
+      <c r="I5" s="26"/>
+      <c r="J5" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="22">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s" s="23">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s" s="23">
-        <v>40</v>
-      </c>
-      <c r="E4" s="24">
-        <f>IF(C4="H",ROUND(B4*K$3,2),B4)</f>
-        <v>19.21</v>
-      </c>
-      <c r="F4" t="s" s="25">
+      <c r="K5" s="34">
+        <v>0.15</v>
+      </c>
+      <c r="L5" s="26"/>
+    </row>
+    <row r="6" spans="1:12" ht="27.3" customHeight="1">
+      <c r="A6" s="35"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="13">
+        <f>IF(C6&lt;&gt;"",ROUND(B6*(VLOOKUP(C6, 'Tax List'!A:B, 2,FALSE)+1),2),B6)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H6" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="26"/>
+      <c r="J6" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+    </row>
+    <row r="7" spans="1:12" ht="27.3" customHeight="1">
+      <c r="A7" s="35"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="13">
+        <f>IF(C7&lt;&gt;"",ROUND(B7*(VLOOKUP(C7, 'Tax List'!A:B, 2,FALSE)+1),2),B7)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="32"/>
+      <c r="G7" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="26"/>
+      <c r="J7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="26">
-        <f>IF(F4="ALL",K$4,LEN(TRIM(F4))-LEN(SUBSTITUTE(TRIM(F4),",",""))+1)</f>
+      <c r="K7" s="28">
+        <f>(SUMIF(F$3:F$8,"ALL",H$3:H$8)+SUMIF(F$3:F$8,"*"&amp;J7&amp;"*",H$3:H$8))*(1+K$5)</f>
+        <v>44.832749999999997</v>
+      </c>
+      <c r="L7" s="26"/>
+    </row>
+    <row r="8" spans="1:12" ht="27.3" customHeight="1">
+      <c r="A8" s="35"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="13">
+        <f>IF(C8&lt;&gt;"",ROUND(B8*(VLOOKUP(C8, 'Tax List'!A:B, 2,FALSE)+1),2),B8)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="24">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H4" s="27">
-        <f>E4/G4</f>
-        <v>19.21</v>
-      </c>
-      <c r="I4" s="28"/>
-      <c r="J4" t="s" s="23">
-        <v>20</v>
-      </c>
-      <c r="K4" s="29">
-        <v>2</v>
-      </c>
-      <c r="L4" s="28"/>
-    </row>
-    <row r="5" ht="27.35" customHeight="1">
-      <c r="A5" t="s" s="21">
-        <v>43</v>
-      </c>
-      <c r="B5" s="22">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s" s="23">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s" s="23">
-        <v>40</v>
-      </c>
-      <c r="E5" s="24">
-        <f>IF(C5="H",ROUND(B5*K$3,2),B5)</f>
-        <v>13.56</v>
-      </c>
-      <c r="F5" t="s" s="25">
-        <v>15</v>
-      </c>
-      <c r="G5" s="26">
-        <f>IF(F5="ALL",K$4,LEN(TRIM(F5))-LEN(SUBSTITUTE(TRIM(F5),",",""))+1)</f>
-        <v>1</v>
-      </c>
-      <c r="H5" s="27">
-        <f>E5/G5</f>
-        <v>13.56</v>
-      </c>
-      <c r="I5" s="28"/>
-      <c r="J5" t="s" s="23">
+      <c r="H8" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="26"/>
+      <c r="J8" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="38">
-        <v>0.15</v>
-      </c>
-      <c r="L5" s="28"/>
-    </row>
-    <row r="6" ht="27.35" customHeight="1">
-      <c r="A6" s="39"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="24">
-        <f>IF(C6="H",ROUND(B6*K$3,2),B6)</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="26">
-        <f>IF(F6="ALL",K$4,LEN(TRIM(F6))-LEN(SUBSTITUTE(TRIM(F6),",",""))+1)</f>
-        <v>1</v>
-      </c>
-      <c r="H6" s="27">
-        <f>E6/G6</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="28"/>
-      <c r="J6" t="s" s="40">
-        <v>45</v>
-      </c>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-    </row>
-    <row r="7" ht="27.35" customHeight="1">
-      <c r="A7" s="39"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="24">
-        <f>IF(C7="H",ROUND(B7*K$3,2),B7)</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="26">
-        <f>IF(F7="ALL",K$4,LEN(TRIM(F7))-LEN(SUBSTITUTE(TRIM(F7),",",""))+1)</f>
-        <v>1</v>
-      </c>
-      <c r="H7" s="27">
-        <f>E7/G7</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="28"/>
-      <c r="J7" t="s" s="23">
-        <v>15</v>
-      </c>
-      <c r="K7" s="30">
-        <f>(SUMIF(F$3:F$8,"ALL",H$3:H$8)+SUMIF(F$3:F$8,"*"&amp;J7&amp;"*",H$3:H$8))*(1+K$5)</f>
-        <v>44.83275</v>
-      </c>
-      <c r="L7" s="28"/>
-    </row>
-    <row r="8" ht="27.35" customHeight="1">
-      <c r="A8" s="39"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="24">
-        <f>IF(C8="H",ROUND(B8*K$3,2),B8)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="26">
-        <f>IF(F8="ALL",K$4,LEN(TRIM(F8))-LEN(SUBSTITUTE(TRIM(F8),",",""))+1)</f>
-        <v>1</v>
-      </c>
-      <c r="H8" s="27">
-        <f>E8/G8</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="28"/>
-      <c r="J8" t="s" s="23">
-        <v>46</v>
-      </c>
-      <c r="K8" s="30">
+      <c r="K8" s="28">
         <f>(SUMIF(F$3:F$8,"ALL",H$3:H$8)+SUMIF(F$3:F$8,"*"&amp;J8&amp;"*",H$3:H$8))*(1+K$5)</f>
-        <v>7.14725</v>
-      </c>
-      <c r="L8" s="28"/>
-    </row>
-    <row r="9" ht="22.95" customHeight="1">
-      <c r="A9" t="s" s="32">
-        <v>28</v>
-      </c>
-      <c r="B9" s="33">
+        <v>7.1472499999999997</v>
+      </c>
+      <c r="L8" s="26"/>
+    </row>
+    <row r="9" spans="1:12" ht="22.95" customHeight="1">
+      <c r="A9" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="30">
         <f>SUM(B3:B8)</f>
         <v>40</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31">
         <f>SUM(E3:E8)</f>
         <v>45.2</v>
       </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="28"/>
-    </row>
-    <row r="10" ht="22.95" customHeight="1">
-      <c r="A10" s="36"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" t="s" s="23">
-        <v>28</v>
-      </c>
-      <c r="K10" s="30">
+      <c r="F9" s="32"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="26"/>
+    </row>
+    <row r="10" spans="1:12" ht="22.95" customHeight="1">
+      <c r="A10" s="33"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="28">
         <f>SUM(K6:K9)</f>
         <v>51.98</v>
       </c>
-      <c r="L10" s="28"/>
+      <c r="L10" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{08DDE6E9-3C0B-481F-875B-C2C050D5304B}">
+          <x14:formula1>
+            <xm:f>'Tax List'!$A$2:$A$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:C8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>